<commit_message>
"Deleted the generated Reports and updated TestData File"
</commit_message>
<xml_diff>
--- a/Driver/InputTestData.xlsx
+++ b/Driver/InputTestData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>${username}</t>
   </si>
@@ -22,6 +22,9 @@
     <t>${error_message}</t>
   </si>
   <si>
+    <t>abcd</t>
+  </si>
+  <si>
     <t>ihjk</t>
   </si>
   <si>
@@ -29,6 +32,9 @@
   </si>
   <si>
     <t>cdef</t>
+  </si>
+  <si>
+    <t>efgh</t>
   </si>
   <si>
     <t>ghij</t>
@@ -104,30 +110,36 @@
       </c>
     </row>
     <row r="2">
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>